<commit_message>
ldm connector switch google code style
</commit_message>
<xml_diff>
--- a/src/main/resources/quality-report-info.xlsx
+++ b/src/main/resources/quality-report-info.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20367"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ad\FS\G230-Home\schmidte\CCP-IT\QB-Generator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\samply.share.client.v2\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2A330E1-A3A4-4AA0-9570-579E8E232996}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="37605" windowHeight="17430"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="37605" windowHeight="17430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -147,19 +148,19 @@
     <t>Die aktuelle Version der "allgemeinen Fehler" finden Sie hier:</t>
   </si>
   <si>
-    <t>https://wiki.mitro.dkfz.de/pages/viewpage.action?pageId=23036372</t>
-  </si>
-  <si>
     <t>Tabs: "filtered elements"; "all elements"</t>
   </si>
   <si>
     <t>Tab: "data element stats"</t>
+  </si>
+  <si>
+    <t>https://wiki.verbis.dkfz.de/pages/viewpage.action?pageId=23036372</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -296,19 +297,9 @@
   </cellStyleXfs>
   <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -354,9 +345,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -365,6 +353,19 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -646,328 +647,328 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="43.28515625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="142" style="2" customWidth="1"/>
-    <col min="3" max="3" width="46.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="2"/>
-    <col min="5" max="5" width="31.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="43.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="142" style="1" customWidth="1"/>
+    <col min="3" max="3" width="46.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="1"/>
+    <col min="5" max="5" width="31.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
+      <c r="A1" s="22"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
     </row>
     <row r="2" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="23"/>
+      <c r="N2" s="23"/>
+      <c r="O2" s="23"/>
+      <c r="P2" s="23"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
+      <c r="A3" s="22"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="22"/>
+      <c r="L3" s="22"/>
+      <c r="M3" s="22"/>
+      <c r="N3" s="22"/>
+      <c r="O3" s="22"/>
+      <c r="P3" s="22"/>
     </row>
     <row r="4" spans="1:16" ht="183.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
-      <c r="P4" s="5"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="25"/>
+      <c r="K4" s="25"/>
+      <c r="L4" s="25"/>
+      <c r="M4" s="25"/>
+      <c r="N4" s="25"/>
+      <c r="O4" s="25"/>
+      <c r="P4" s="25"/>
     </row>
     <row r="5" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="6" spans="1:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="A6" s="6"/>
+      <c r="A6" s="2"/>
     </row>
     <row r="7" spans="1:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="A7" s="6"/>
-    </row>
-    <row r="8" spans="1:16" s="8" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="7" t="s">
+      <c r="A7" s="2"/>
+    </row>
+    <row r="8" spans="1:16" s="4" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="8" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="8" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="8" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="8" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="8" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="8" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="13" t="s">
+      <c r="A16" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="10" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="26" t="s">
+      <c r="A17" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="8"/>
+    </row>
+    <row r="18" spans="1:16" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A18" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A19" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" s="13" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="B17" s="12"/>
-    </row>
-    <row r="18" spans="1:16" s="17" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A18" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" s="17" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A19" s="18" t="s">
+      <c r="B21" s="15"/>
+    </row>
+    <row r="22" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A24" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A25" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="19" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="20" t="s">
+      <c r="B25" s="15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="21" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" s="17" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="26" t="s">
+      <c r="B26" s="17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+      <c r="A27" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+      <c r="A28" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+      <c r="A30" s="2"/>
+    </row>
+    <row r="31" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+      <c r="A31" s="2"/>
+    </row>
+    <row r="32" spans="1:16" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="A32" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="B32" s="26"/>
+      <c r="C32" s="26"/>
+      <c r="D32" s="26"/>
+      <c r="E32" s="26"/>
+      <c r="F32" s="26"/>
+      <c r="G32" s="26"/>
+      <c r="H32" s="26"/>
+      <c r="I32" s="26"/>
+      <c r="J32" s="26"/>
+      <c r="K32" s="26"/>
+      <c r="L32" s="26"/>
+      <c r="M32" s="26"/>
+      <c r="N32" s="26"/>
+      <c r="O32" s="26"/>
+      <c r="P32" s="26"/>
+    </row>
+    <row r="33" spans="1:16" customFormat="1" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="A33" s="18"/>
+      <c r="B33" s="18"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
+      <c r="H33" s="18"/>
+      <c r="I33" s="18"/>
+      <c r="J33" s="18"/>
+      <c r="K33" s="18"/>
+      <c r="L33" s="18"/>
+      <c r="M33" s="18"/>
+      <c r="N33" s="18"/>
+      <c r="O33" s="18"/>
+      <c r="P33" s="18"/>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F34" s="19"/>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A35" s="20" t="s">
         <v>40</v>
-      </c>
-      <c r="B21" s="19"/>
-    </row>
-    <row r="22" spans="1:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="A22" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23" s="14" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" s="17" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A24" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="B24" s="16" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" s="17" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A25" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="B25" s="19" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="B26" s="21" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="A27" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="A28" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B28" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="B29" s="14" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="A30" s="6"/>
-    </row>
-    <row r="31" spans="1:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="A31" s="6"/>
-    </row>
-    <row r="32" spans="1:16" ht="18.75" x14ac:dyDescent="0.2">
-      <c r="A32" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="B32" s="22"/>
-      <c r="C32" s="22"/>
-      <c r="D32" s="22"/>
-      <c r="E32" s="22"/>
-      <c r="F32" s="22"/>
-      <c r="G32" s="22"/>
-      <c r="H32" s="22"/>
-      <c r="I32" s="22"/>
-      <c r="J32" s="22"/>
-      <c r="K32" s="22"/>
-      <c r="L32" s="22"/>
-      <c r="M32" s="22"/>
-      <c r="N32" s="22"/>
-      <c r="O32" s="22"/>
-      <c r="P32" s="22"/>
-    </row>
-    <row r="33" spans="1:16" customFormat="1" ht="18.75" x14ac:dyDescent="0.2">
-      <c r="A33" s="23"/>
-      <c r="B33" s="23"/>
-      <c r="C33" s="23"/>
-      <c r="D33" s="23"/>
-      <c r="E33" s="23"/>
-      <c r="F33" s="23"/>
-      <c r="G33" s="23"/>
-      <c r="H33" s="23"/>
-      <c r="I33" s="23"/>
-      <c r="J33" s="23"/>
-      <c r="K33" s="23"/>
-      <c r="L33" s="23"/>
-      <c r="M33" s="23"/>
-      <c r="N33" s="23"/>
-      <c r="O33" s="23"/>
-      <c r="P33" s="23"/>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A34" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F34" s="24"/>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A35" s="25" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -979,7 +980,7 @@
     <mergeCell ref="A32:P32"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A35" r:id="rId1"/>
+    <hyperlink ref="A35" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
Quality Report Info Sheet: CCP-Office as contact
</commit_message>
<xml_diff>
--- a/src/main/resources/quality-report-info.xlsx
+++ b/src/main/resources/quality-report-info.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20367"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20375"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\samply.share.client.v2\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\share-client\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2A330E1-A3A4-4AA0-9570-579E8E232996}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF1A65E4-979A-433E-AA7C-1663C3D784BA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="37605" windowHeight="17430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,6 +30,123 @@
     <t>Qualitätsbericht aus Brückenkopf</t>
   </si>
   <si>
+    <t>Erläuterung zu den Spalten des Qualitätsberichts</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>Datenelement + Link zur Beschreibung des Datenelements im MDR Repository</t>
+  </si>
+  <si>
+    <t>DKTK-id</t>
+  </si>
+  <si>
+    <t>Identifikator im MDR</t>
+  </si>
+  <si>
+    <t>dataelement MDR</t>
+  </si>
+  <si>
+    <t>Name des Datenelementes nach MDR</t>
+  </si>
+  <si>
+    <t>dataelement CXX</t>
+  </si>
+  <si>
+    <t>Name des Datenelementes nach CentraXX</t>
+  </si>
+  <si>
+    <t>datatype MDR</t>
+  </si>
+  <si>
+    <t>Datentyp des Datenelementes im MDR</t>
+  </si>
+  <si>
+    <t>value MDR</t>
+  </si>
+  <si>
+    <t>Name der Ausprägung nach MDR</t>
+  </si>
+  <si>
+    <t>value CXX</t>
+  </si>
+  <si>
+    <t>Name der Ausprägung nach CentraXX</t>
+  </si>
+  <si>
+    <t>validation</t>
+  </si>
+  <si>
+    <t>Validierung der Ausprägung gegen MDR-Definition</t>
+  </si>
+  <si>
+    <t>number of patients CXX</t>
+  </si>
+  <si>
+    <t>Anzahl von Patienten in CentraXX mit dieser Datenelement-Ausprägung</t>
+  </si>
+  <si>
+    <t>% of patients with entry for this element</t>
+  </si>
+  <si>
+    <t>Anteil der Patienten mit dieser Datenelement-Ausprägung an allen Patienten, für die überhaupt eine Ausprägung vorliegt</t>
+  </si>
+  <si>
+    <t>% of patients - total</t>
+  </si>
+  <si>
+    <t>Anteil der Patienten mit dieser Datenelement-Ausprägung an der Gesamtzahl der Patienten</t>
+  </si>
+  <si>
+    <t>Number of patients with entry for this element</t>
+  </si>
+  <si>
+    <t>Anzahl von Patienten, für die eine Ausprägung für dieses Datenelement vorliegt</t>
+  </si>
+  <si>
+    <t>Anteil der Patienten, für die eine Ausprägung für dieses Datenelement vorliegt, an der Gesamtzahl der Patienten</t>
+  </si>
+  <si>
+    <t>Number of patients with match only</t>
+  </si>
+  <si>
+    <t>Anzahl von Patienten, für die nur MDR-konforme Ausprägungen vorliegen</t>
+  </si>
+  <si>
+    <t>Anteil der Patienten, für die nur MDR-konforme Ausprägungen vorliegen, an allen Patienten, für die überhaupt eine Ausprägung vorliegt</t>
+  </si>
+  <si>
+    <t>Anteil der Patienten, für die nur MDR-konforme Ausprägungen vorliegen, an der Gesamtzahl der Patienten</t>
+  </si>
+  <si>
+    <t>Number of patients with any mismatch</t>
+  </si>
+  <si>
+    <t>Anzahl von Patienten, für die mindestens eine nicht-MDR-konforme Ausprägung vorliegt</t>
+  </si>
+  <si>
+    <t>Anteil der Patienten, für die mindestens eine nicht-MDR-konforme Ausprägung vorliegt, an allen Patienten, für die überhaupt eine Ausprägung vorliegt</t>
+  </si>
+  <si>
+    <t>Anteil der Patienten, für die mindestens eine nicht-MDR-konforme Ausprägung vorliegt, an der Gesamtzahl der Patienten</t>
+  </si>
+  <si>
+    <t>Auflistung bekannter „allgemeiner Fehler“, die nicht vom Standort bearbeitet werden müssen:</t>
+  </si>
+  <si>
+    <t>Die aktuelle Version der "allgemeinen Fehler" finden Sie hier:</t>
+  </si>
+  <si>
+    <t>Tabs: "filtered elements"; "all elements"</t>
+  </si>
+  <si>
+    <t>Tab: "data element stats"</t>
+  </si>
+  <si>
+    <t>https://wiki.verbis.dkfz.de/pages/viewpage.action?pageId=23036372</t>
+  </si>
+  <si>
     <t>Dieser Qualitätsbericht wurde automatisch erstellt über die Teilerfunktion „Qualitätsbericht erstellen“.
 Einige Hinweise zur Nutzung dieses Berichts:
 1. Grundlage der Erstellung dieses Qualitätsberichts (QB) ist ein Abgleich der von CentraXX ausgegebenen Daten (Elemente und ihre Ausprägungen) mit den im MDS/MDR definierten Datenelementen und Ausprägungen. Für die klinischen Daten wurden hierfür z.B. die Werte gemäß des ADT 2014 und der TNM-Klassifikationen verwendet.
@@ -37,124 +154,7 @@
 3. Die rot markierten Reihen weisen auf Abweichungen der Daten in Bezug auf die im MDR definierten Formate und Begriffe hin.
 4. Im Qualitätsbericht der aktuellen Version werden auch schon bekannte, aber noch nicht behobene „allgemeine“, also nicht standort-spezifische Fehler aufgelistet. Diese bekannten Fehler sind unten benannt – diese können also bei der Bearbeitung der Abweichungen ignoriert werden.
 5. Um die Standorte zu unterstützen, bietet das CCP Office Ihnen an, den QB auf reine Datenerfassungs-Abweichungen zu sichten. I.d.R. sind dies Dokumentationsfehler, es können aber auch bewusste lokale Modifikationen der Daten sein, die von der Tumordokumentation (resp. Biobank) erfasst werden.
-Bei Fragen zu technischen Aspekten im Zusammenhang mit dem QB wenden Sie sich bitte an Herrn Juarez, bei generellen und inhaltlichen Fragen wenden Sie sich bitte an Kristina Ihrig.</t>
-  </si>
-  <si>
-    <t>Erläuterung zu den Spalten des Qualitätsberichts</t>
-  </si>
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>Datenelement + Link zur Beschreibung des Datenelements im MDR Repository</t>
-  </si>
-  <si>
-    <t>DKTK-id</t>
-  </si>
-  <si>
-    <t>Identifikator im MDR</t>
-  </si>
-  <si>
-    <t>dataelement MDR</t>
-  </si>
-  <si>
-    <t>Name des Datenelementes nach MDR</t>
-  </si>
-  <si>
-    <t>dataelement CXX</t>
-  </si>
-  <si>
-    <t>Name des Datenelementes nach CentraXX</t>
-  </si>
-  <si>
-    <t>datatype MDR</t>
-  </si>
-  <si>
-    <t>Datentyp des Datenelementes im MDR</t>
-  </si>
-  <si>
-    <t>value MDR</t>
-  </si>
-  <si>
-    <t>Name der Ausprägung nach MDR</t>
-  </si>
-  <si>
-    <t>value CXX</t>
-  </si>
-  <si>
-    <t>Name der Ausprägung nach CentraXX</t>
-  </si>
-  <si>
-    <t>validation</t>
-  </si>
-  <si>
-    <t>Validierung der Ausprägung gegen MDR-Definition</t>
-  </si>
-  <si>
-    <t>number of patients CXX</t>
-  </si>
-  <si>
-    <t>Anzahl von Patienten in CentraXX mit dieser Datenelement-Ausprägung</t>
-  </si>
-  <si>
-    <t>% of patients with entry for this element</t>
-  </si>
-  <si>
-    <t>Anteil der Patienten mit dieser Datenelement-Ausprägung an allen Patienten, für die überhaupt eine Ausprägung vorliegt</t>
-  </si>
-  <si>
-    <t>% of patients - total</t>
-  </si>
-  <si>
-    <t>Anteil der Patienten mit dieser Datenelement-Ausprägung an der Gesamtzahl der Patienten</t>
-  </si>
-  <si>
-    <t>Number of patients with entry for this element</t>
-  </si>
-  <si>
-    <t>Anzahl von Patienten, für die eine Ausprägung für dieses Datenelement vorliegt</t>
-  </si>
-  <si>
-    <t>Anteil der Patienten, für die eine Ausprägung für dieses Datenelement vorliegt, an der Gesamtzahl der Patienten</t>
-  </si>
-  <si>
-    <t>Number of patients with match only</t>
-  </si>
-  <si>
-    <t>Anzahl von Patienten, für die nur MDR-konforme Ausprägungen vorliegen</t>
-  </si>
-  <si>
-    <t>Anteil der Patienten, für die nur MDR-konforme Ausprägungen vorliegen, an allen Patienten, für die überhaupt eine Ausprägung vorliegt</t>
-  </si>
-  <si>
-    <t>Anteil der Patienten, für die nur MDR-konforme Ausprägungen vorliegen, an der Gesamtzahl der Patienten</t>
-  </si>
-  <si>
-    <t>Number of patients with any mismatch</t>
-  </si>
-  <si>
-    <t>Anzahl von Patienten, für die mindestens eine nicht-MDR-konforme Ausprägung vorliegt</t>
-  </si>
-  <si>
-    <t>Anteil der Patienten, für die mindestens eine nicht-MDR-konforme Ausprägung vorliegt, an allen Patienten, für die überhaupt eine Ausprägung vorliegt</t>
-  </si>
-  <si>
-    <t>Anteil der Patienten, für die mindestens eine nicht-MDR-konforme Ausprägung vorliegt, an der Gesamtzahl der Patienten</t>
-  </si>
-  <si>
-    <t>Auflistung bekannter „allgemeiner Fehler“, die nicht vom Standort bearbeitet werden müssen:</t>
-  </si>
-  <si>
-    <t>Die aktuelle Version der "allgemeinen Fehler" finden Sie hier:</t>
-  </si>
-  <si>
-    <t>Tabs: "filtered elements"; "all elements"</t>
-  </si>
-  <si>
-    <t>Tab: "data element stats"</t>
-  </si>
-  <si>
-    <t>https://wiki.verbis.dkfz.de/pages/viewpage.action?pageId=23036372</t>
+Bei Fragen zu technischen Aspekten im Zusammenhang mit dem QB wenden Sie sich bitte an Herrn Juarez, bei generellen und inhaltlichen Fragen wenden Sie sich bitte an das CCP-Office.</t>
   </si>
 </sst>
 </file>
@@ -651,7 +651,7 @@
   <dimension ref="A1:P35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -722,7 +722,7 @@
     </row>
     <row r="4" spans="1:16" ht="183.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="24" t="s">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="B4" s="25"/>
       <c r="C4" s="25"/>
@@ -749,171 +749,171 @@
     </row>
     <row r="8" spans="1:16" s="4" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>3</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="8" t="s">
         <v>5</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="8" t="s">
         <v>7</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="8" t="s">
         <v>9</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="8" t="s">
         <v>11</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="8" t="s">
         <v>13</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="10" t="s">
         <v>17</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B17" s="8"/>
     </row>
     <row r="18" spans="1:16" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="12" t="s">
         <v>19</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="15" t="s">
         <v>21</v>
-      </c>
-      <c r="B19" s="15" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:16" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="17" t="s">
         <v>23</v>
-      </c>
-      <c r="B20" s="17" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="13" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B21" s="15"/>
     </row>
     <row r="22" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="6" t="s">
         <v>25</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" s="12" t="s">
         <v>28</v>
-      </c>
-      <c r="B24" s="12" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A25" s="14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:16" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" s="6" t="s">
         <v>32</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="28" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="30" spans="1:16" ht="15" x14ac:dyDescent="0.2">
@@ -924,7 +924,7 @@
     </row>
     <row r="32" spans="1:16" ht="18.75" x14ac:dyDescent="0.2">
       <c r="A32" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B32" s="26"/>
       <c r="C32" s="26"/>
@@ -962,13 +962,13 @@
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F34" s="19"/>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A35" s="20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>